<commit_message>
update 9 march 2020
</commit_message>
<xml_diff>
--- a/UpdateFileTest.xlsx
+++ b/UpdateFileTest.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="MydataSheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="LoginSheet" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Sumit</t>
   </si>
@@ -28,28 +29,34 @@
     <t xml:space="preserve">Kumar</t>
   </si>
   <si>
-    <t>The Passionate Programmer</t>
-  </si>
-  <si>
-    <t>Chad Fowler</t>
-  </si>
-  <si>
-    <t>Software Craftmanship</t>
-  </si>
-  <si>
-    <t>Pete McBreen</t>
-  </si>
-  <si>
-    <t>The Art of Agile Development</t>
-  </si>
-  <si>
-    <t>James Shore</t>
-  </si>
-  <si>
-    <t>Continuous Delivery</t>
-  </si>
-  <si>
-    <t>Jez Humble</t>
+    <t xml:space="preserve">The Passionate Programmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chad Fowler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Craftmanship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pete McBreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Art of Agile Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Shore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continuous Delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jez Humble</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0tp</t>
   </si>
 </sst>
 </file>
@@ -64,6 +71,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -147,11 +155,11 @@
   </sheetPr>
   <dimension ref="A2:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -167,60 +175,60 @@
         <v>9971458090</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="n">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D3" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="n">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D4" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="n">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D5" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="n">
-        <v>41.0</v>
+      <c r="D6" s="0" t="n">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -232,4 +240,44 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>9971458090</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>